<commit_message>
3rd Commit. properties tag added in pom.xml to avoide compilation error in maven
</commit_message>
<xml_diff>
--- a/Test_Data/validateAdvancedSearch.xlsx
+++ b/Test_Data/validateAdvancedSearch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ajay\Java_Folder\Java_Eclips\vTiger\Test_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0048E20-DCED-424C-AB1B-E3A49CD4B379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C68BF9F-E618-44E7-9108-6CD87394F212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{9EF757C6-8C73-4F43-9CD6-689675FD6373}"/>
   </bookViews>
@@ -428,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ECC214C-1D02-466D-B7C4-EDBDBB524589}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -472,6 +472,14 @@
         <v>1</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -482,7 +490,7 @@
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -516,9 +524,7 @@
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="A6" s="1"/>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>

</xml_diff>